<commit_message>
Fixed The Problem When Sender Is Not Correct
</commit_message>
<xml_diff>
--- a/email.xlsx
+++ b/email.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Reza</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t xml:space="preserve">globaladlist24@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mahmudul</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mahmudul5809@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -226,7 +232,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -274,6 +280,14 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
@@ -282,6 +296,7 @@
     <hyperlink ref="B3" r:id="rId3" display="thehidepage@gmail.com"/>
     <hyperlink ref="B4" r:id="rId4" display="fgfgytrytu6@gmail.com"/>
     <hyperlink ref="B5" r:id="rId5" display="globaladlist24@gmail.com"/>
+    <hyperlink ref="B6" r:id="rId6" display="mahmudul5809@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>